<commit_message>
Updated for Fall 2025
</commit_message>
<xml_diff>
--- a/residents.xlsx
+++ b/residents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettmanaster/GeorgiaTech/RA/interactions_spring_25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\interactions_fall_25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39444472-BB3E-524D-964A-47E1ACC79F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F9EEAA-B72E-4088-B0AF-053A2117DBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16700" xr2:uid="{09AFDB0D-1FC0-0E40-9DEE-F8D7DA441309}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09AFDB0D-1FC0-0E40-9DEE-F8D7DA441309}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>&lt;List All Residents, ensuring correct spelling&gt;</t>
   </si>
   <si>
-    <t>&lt;mm-DD-YYYY&gt;</t>
-  </si>
-  <si>
     <t>&lt;Description of Interaction&gt;</t>
   </si>
   <si>
@@ -87,16 +84,26 @@
   </si>
   <si>
     <t>Emotional</t>
+  </si>
+  <si>
+    <t>&lt;mm/DD/YYYY&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,23 +468,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059D8599-A6D6-B542-9C0C-62C7D67718AC}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="36.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,61 +498,229 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-      <c r="F3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F4" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F6" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>